<commit_message>
Added Extent reports, screenCapture and Select methods
</commit_message>
<xml_diff>
--- a/SeleniumAutomation_Ascendum/src/main/java/com/qa/ascendum/resources/dataDrivenTest.xlsx
+++ b/SeleniumAutomation_Ascendum/src/main/java/com/qa/ascendum/resources/dataDrivenTest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="24">
   <si>
     <t>C</t>
   </si>
@@ -419,7 +419,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>